<commit_message>
Bulk import almost done, need to test tickets now
</commit_message>
<xml_diff>
--- a/Aardvark/Template.xlsx
+++ b/Aardvark/Template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="145">
   <si>
     <t>FirstName</t>
   </si>
@@ -192,24 +192,9 @@
     <t>; information is not entered; it will reject entries that already exist. Default values will be entered</t>
   </si>
   <si>
-    <t>; as explained below.</t>
-  </si>
-  <si>
     <t>; You will note that any line starting with a semi-colon will be skipped, treated as a comment. This</t>
   </si>
   <si>
-    <t>; allows you to easily "comment out" a line within a section, if needed. The sections below are listed</t>
-  </si>
-  <si>
-    <t>; in this sequence: #Users, #Projects, #ProjectDevelopers, and #Tickets. All the information can be</t>
-  </si>
-  <si>
-    <t>; edited by Aardvark if needed, after the bulk operation completes. A message at the end of the</t>
-  </si>
-  <si>
-    <t>; operation will indicate any records that had to be skipped.</t>
-  </si>
-  <si>
     <t>; Please do not change the sequence of the sections below. You need not use all of them; you can</t>
   </si>
   <si>
@@ -240,15 +225,6 @@
     <t>; The ProjectDevelopers Section</t>
   </si>
   <si>
-    <t>; ProjectName must be a valid name of a Project in the database (or listed above -- which means it will</t>
-  </si>
-  <si>
-    <t>; have just been inserted into the database). DeveloperUserName is required and must be a UserName</t>
-  </si>
-  <si>
-    <t>; having a role of Developer. The same Developer can be listed for multiple Projects.</t>
-  </si>
-  <si>
     <t>; The Tickets Section</t>
   </si>
   <si>
@@ -360,9 +336,6 @@
     <t>; DisplayName optional -- will default to UserName if blank.</t>
   </si>
   <si>
-    <t>; Each User must have a unique UserName -- will be rejected if already in database.</t>
-  </si>
-  <si>
     <t>; Put Y in role column if User is to have that role; multiple roles are permitted.</t>
   </si>
   <si>
@@ -403,6 +376,81 @@
   </si>
   <si>
     <t>Jimmy@me.com</t>
+  </si>
+  <si>
+    <t>SkillLevel</t>
+  </si>
+  <si>
+    <t>; There are three possible skill levels: Junior, Mid-Level, or Senior. Junior is default if no other value</t>
+  </si>
+  <si>
+    <t>Kermit</t>
+  </si>
+  <si>
+    <t>The Frog</t>
+  </si>
+  <si>
+    <t>Kirmy</t>
+  </si>
+  <si>
+    <t>KirmetTheFrog@me.com</t>
+  </si>
+  <si>
+    <t>; Each User must have a unique UserName -- will be skipped over if already in database.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">; allows you to easily "comment out" a line within a section, if needed (these instruction lines are </t>
+  </si>
+  <si>
+    <t xml:space="preserve">; commented out). The following sections are available: #Users, #Projects, #ProjectDevelopers, </t>
+  </si>
+  <si>
+    <t>; and #Tickets. There is "dummy" information that shows the proper format; this can be edited and/or</t>
+  </si>
+  <si>
+    <t>;  removed as needed. You can enter as many new rows as you like. If there are any errors, appropriate</t>
+  </si>
+  <si>
+    <t>; messages will be added to the Log file.</t>
+  </si>
+  <si>
+    <t>; as explained below. Please to not use any double quotes in any column.</t>
+  </si>
+  <si>
+    <t>; ProjectName and Description must be an exact match for a ProjectName/Description of a Project in</t>
+  </si>
+  <si>
+    <t>;the database (or listed above -- which means it will have just been inserted into the database).</t>
+  </si>
+  <si>
+    <t>; DeveloperUserName is required and must be a UserName having a role of Developer. The same</t>
+  </si>
+  <si>
+    <t>; DeveloperUserName can be listed for multiple Projects.</t>
+  </si>
+  <si>
+    <t>; A Project can occur only once in this section (with only one ProjectManagerUserName).</t>
+  </si>
+  <si>
+    <t>; A Project can occur multiple times in this section (this allows more than one DeveloperUserName</t>
+  </si>
+  <si>
+    <t>; the same.</t>
+  </si>
+  <si>
+    <t>; to be listed). Each time the same Project is listed, its Name and Description must be repeated exactly</t>
+  </si>
+  <si>
+    <t>ProjectDescription</t>
+  </si>
+  <si>
+    <t>Annoying sounds</t>
+  </si>
+  <si>
+    <t>Chirps quite loudly</t>
+  </si>
+  <si>
+    <t>; ProjectDescription is also required to uniquely identify the Project this belongs to; if no match, no Project will be specified</t>
   </si>
 </sst>
 </file>
@@ -775,11 +823,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L85"/>
+  <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F41" sqref="F41"/>
+      <selection pane="topRight" activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,973 +841,1222 @@
     <col min="7" max="7" width="14.5703125" style="5" customWidth="1"/>
     <col min="8" max="8" width="17.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14.5703125" style="5" customWidth="1"/>
-    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="5" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G1"/>
       <c r="H1"/>
       <c r="I1"/>
-      <c r="J1"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G2"/>
       <c r="H2"/>
       <c r="I2"/>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>53</v>
       </c>
       <c r="G3"/>
       <c r="H3"/>
       <c r="I3"/>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>54</v>
       </c>
       <c r="G4"/>
       <c r="H4"/>
       <c r="I4"/>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>55</v>
       </c>
       <c r="G5"/>
       <c r="H5"/>
       <c r="I5"/>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="G6"/>
       <c r="H6"/>
       <c r="I6"/>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>56</v>
       </c>
       <c r="G7"/>
       <c r="H7"/>
       <c r="I7"/>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>57</v>
       </c>
       <c r="G8"/>
       <c r="H8"/>
       <c r="I8"/>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>132</v>
       </c>
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
-      <c r="J9"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>47</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
-      <c r="J10"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11"/>
       <c r="H11"/>
       <c r="I11"/>
-      <c r="J11"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
       <c r="G12"/>
       <c r="H12"/>
       <c r="I12"/>
-      <c r="J12"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>128</v>
       </c>
       <c r="G13"/>
       <c r="H13"/>
       <c r="I13"/>
-      <c r="J13"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>129</v>
       </c>
       <c r="G14"/>
       <c r="H14"/>
       <c r="I14"/>
-      <c r="J14"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
-      <c r="J15"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
       <c r="G16"/>
       <c r="H16"/>
       <c r="I16"/>
-      <c r="J16"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="G17"/>
       <c r="H17"/>
       <c r="I17"/>
-      <c r="J17"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="G18"/>
       <c r="H18"/>
       <c r="I18"/>
-      <c r="J18"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="G19"/>
       <c r="H19"/>
       <c r="I19"/>
-      <c r="J19"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="G20"/>
       <c r="H20"/>
       <c r="I20"/>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G21"/>
       <c r="H21"/>
       <c r="I21"/>
-      <c r="J21"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="G22"/>
       <c r="H22"/>
       <c r="I22"/>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="G23"/>
       <c r="H23"/>
       <c r="I23"/>
-      <c r="J23"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G24"/>
       <c r="H24"/>
       <c r="I24"/>
-      <c r="J24"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>62</v>
       </c>
       <c r="G25"/>
       <c r="H25"/>
       <c r="I25"/>
-      <c r="J25"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>47</v>
       </c>
       <c r="G26"/>
       <c r="H26"/>
       <c r="I26"/>
-      <c r="J26"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="G27"/>
       <c r="H27"/>
       <c r="I27"/>
-      <c r="J27"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G28"/>
       <c r="H28"/>
       <c r="I28"/>
-      <c r="J28"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="G29"/>
       <c r="H29"/>
       <c r="I29"/>
-      <c r="J29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="G30"/>
       <c r="H30"/>
       <c r="I30"/>
-      <c r="J30"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="G31"/>
       <c r="H31"/>
       <c r="I31"/>
-      <c r="J31"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="G32"/>
       <c r="H32"/>
       <c r="I32"/>
-      <c r="J32"/>
-    </row>
-    <row r="33" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="6"/>
-      <c r="H33" s="6"/>
-      <c r="I33" s="6"/>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+    </row>
+    <row r="34" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
       <c r="I34" s="6"/>
       <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
       <c r="I35" s="6"/>
       <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="6"/>
       <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="G37" s="6"/>
       <c r="H37" s="6"/>
       <c r="I37" s="6"/>
       <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="6"/>
       <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+    </row>
+    <row r="39" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+    </row>
+    <row r="41" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-    </row>
-    <row r="40" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E42" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="G42" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G40" s="4" t="s">
+      <c r="H42" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="I40" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="J40" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K40" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" t="s">
-        <v>127</v>
-      </c>
-      <c r="D41" t="s">
-        <v>127</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F41" t="s">
-        <v>109</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I41" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B42" t="s">
-        <v>31</v>
-      </c>
-      <c r="C42" t="s">
-        <v>30</v>
-      </c>
-      <c r="D42" t="s">
-        <v>30</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F42" t="s">
-        <v>110</v>
-      </c>
-      <c r="I42" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="M42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>6</v>
+        <v>116</v>
       </c>
       <c r="B43" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="C43" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="D43" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F43" t="s">
-        <v>111</v>
+        <v>118</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G43" t="s">
+        <v>101</v>
       </c>
       <c r="H43" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J43" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>30</v>
+      </c>
+      <c r="B44" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" t="s">
+        <v>30</v>
+      </c>
+      <c r="D44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E44" t="s">
+        <v>84</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G44" t="s">
+        <v>102</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>7</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G45" t="s">
+        <v>103</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>11</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C46" t="s">
         <v>22</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>10</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="E46" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H44" s="5" t="s">
+      <c r="G46"/>
+      <c r="I46" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="J46" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>27</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>28</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C47" t="s">
         <v>27</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D47" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="E47" t="s">
+        <v>98</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J45" s="5" t="s">
+      <c r="G47"/>
+      <c r="K47" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>122</v>
+      </c>
+      <c r="B48" t="s">
+        <v>123</v>
+      </c>
+      <c r="C48" t="s">
+        <v>124</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>47</v>
       </c>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>69</v>
-      </c>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>64</v>
+      </c>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G48" s="6"/>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="6"/>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-    </row>
-    <row r="51" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="G51" s="6"/>
       <c r="H51" s="6"/>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+    </row>
+    <row r="52" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+    </row>
+    <row r="53" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+      <c r="K53" s="6"/>
+      <c r="L53" s="6"/>
+      <c r="M53" s="6"/>
+    </row>
+    <row r="54" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+    </row>
+    <row r="55" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+    </row>
+    <row r="56" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
-      <c r="J52" s="4"/>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="2" t="s">
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+    </row>
+    <row r="57" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B57" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C57" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>19</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B58" t="s">
         <v>20</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C58" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>25</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B59" t="s">
         <v>26</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C59" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-    </row>
-    <row r="59" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G59" s="6"/>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-    </row>
-    <row r="60" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="G60" s="6"/>
-      <c r="H60" s="6"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="6"/>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="2" t="s">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+    </row>
+    <row r="63" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+    </row>
+    <row r="64" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
+      <c r="L64" s="6"/>
+      <c r="M64" s="6"/>
+    </row>
+    <row r="65" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+      <c r="K65" s="6"/>
+      <c r="L65" s="6"/>
+      <c r="M65" s="6"/>
+    </row>
+    <row r="66" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+    </row>
+    <row r="67" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+    </row>
+    <row r="68" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="4"/>
+      <c r="L68" s="4"/>
+      <c r="M68" s="4"/>
+    </row>
+    <row r="69" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+    </row>
+    <row r="70" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="4"/>
+      <c r="L70" s="4"/>
+      <c r="M70" s="4"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" t="s">
+        <v>20</v>
+      </c>
+      <c r="C71" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>19</v>
+      </c>
+      <c r="B72" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>25</v>
+      </c>
+      <c r="B73" t="s">
+        <v>26</v>
+      </c>
+      <c r="C73" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>47</v>
       </c>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
-      <c r="J61" s="4"/>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
-      <c r="J62" s="4"/>
-    </row>
-    <row r="63" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
-      <c r="J63" s="4"/>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>19</v>
-      </c>
-      <c r="B64" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>19</v>
-      </c>
-      <c r="B65" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>25</v>
-      </c>
-      <c r="B66" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="G69" s="6"/>
-      <c r="H69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-    </row>
-    <row r="70" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="G70" s="6"/>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-    </row>
-    <row r="71" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="G71" s="6"/>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-    </row>
-    <row r="72" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G72" s="6"/>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-    </row>
-    <row r="73" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="G73" s="6"/>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-    </row>
-    <row r="74" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G74" s="6"/>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-    </row>
-    <row r="75" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G75" s="6"/>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-    </row>
-    <row r="76" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G76" s="6"/>
       <c r="H76" s="6"/>
       <c r="I76" s="6"/>
       <c r="J76" s="6"/>
-    </row>
-    <row r="77" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K76" s="6"/>
+      <c r="L76" s="6"/>
+      <c r="M76" s="6"/>
+    </row>
+    <row r="77" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G77" s="6"/>
       <c r="H77" s="6"/>
       <c r="I77" s="6"/>
       <c r="J77" s="6"/>
-    </row>
-    <row r="78" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K77" s="6"/>
+      <c r="L77" s="6"/>
+      <c r="M77" s="6"/>
+    </row>
+    <row r="78" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G78" s="6"/>
       <c r="H78" s="6"/>
       <c r="I78" s="6"/>
       <c r="J78" s="6"/>
-    </row>
-    <row r="79" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K78" s="6"/>
+      <c r="L78" s="6"/>
+      <c r="M78" s="6"/>
+    </row>
+    <row r="79" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>103</v>
+        <v>144</v>
       </c>
       <c r="G79" s="6"/>
       <c r="H79" s="6"/>
       <c r="I79" s="6"/>
       <c r="J79" s="6"/>
-    </row>
-    <row r="80" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K79" s="6"/>
+      <c r="L79" s="6"/>
+      <c r="M79" s="6"/>
+    </row>
+    <row r="80" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="G80" s="6"/>
       <c r="H80" s="6"/>
       <c r="I80" s="6"/>
       <c r="J80" s="6"/>
-    </row>
-    <row r="81" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
+      <c r="K80" s="6"/>
+      <c r="L80" s="6"/>
+      <c r="M80" s="6"/>
+    </row>
+    <row r="81" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+      <c r="K81" s="6"/>
+      <c r="L81" s="6"/>
+      <c r="M81" s="6"/>
+    </row>
+    <row r="82" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+      <c r="K82" s="6"/>
+      <c r="L82" s="6"/>
+      <c r="M82" s="6"/>
+    </row>
+    <row r="83" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+      <c r="K83" s="6"/>
+      <c r="L83" s="6"/>
+      <c r="M83" s="6"/>
+    </row>
+    <row r="84" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+      <c r="K84" s="6"/>
+      <c r="L84" s="6"/>
+      <c r="M84" s="6"/>
+    </row>
+    <row r="85" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
+      <c r="L85" s="6"/>
+      <c r="M85" s="6"/>
+    </row>
+    <row r="86" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+      <c r="K86" s="6"/>
+      <c r="L86" s="6"/>
+      <c r="M86" s="6"/>
+    </row>
+    <row r="87" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+    </row>
+    <row r="88" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+      <c r="K88" s="6"/>
+      <c r="L88" s="6"/>
+      <c r="M88" s="6"/>
+    </row>
+    <row r="89" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-      <c r="J81" s="4"/>
-    </row>
-    <row r="82" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="2" t="s">
+      <c r="G89" s="4"/>
+      <c r="H89" s="4"/>
+      <c r="I89" s="4"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="4"/>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+    </row>
+    <row r="90" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B90" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C82" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D82" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="E90" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F90" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="G90" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G82" s="4" t="s">
+      <c r="H90" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H82" s="4" t="s">
+      <c r="I90" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I82" s="4" t="s">
+      <c r="J90" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K90" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K82" s="4" t="s">
+      <c r="L90" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L82" s="4" t="s">
+      <c r="M90" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" t="s">
+        <v>80</v>
+      </c>
+      <c r="C91" t="s">
+        <v>81</v>
+      </c>
+      <c r="D91" t="s">
+        <v>19</v>
+      </c>
+      <c r="E91" t="s">
+        <v>20</v>
+      </c>
+      <c r="F91" t="s">
+        <v>27</v>
+      </c>
+      <c r="G91" t="s">
+        <v>30</v>
+      </c>
+      <c r="H91" s="7">
+        <v>42277</v>
+      </c>
+      <c r="I91" s="5">
+        <v>5</v>
+      </c>
+      <c r="J91" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="K91" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L91" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="M91" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B92" t="s">
+        <v>86</v>
+      </c>
+      <c r="C92" s="8">
+        <v>42216</v>
+      </c>
+      <c r="D92" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" t="s">
+        <v>20</v>
+      </c>
+      <c r="F92" t="s">
+        <v>22</v>
+      </c>
+      <c r="G92"/>
+      <c r="H92" s="7">
+        <v>42247</v>
+      </c>
+      <c r="I92" s="5">
+        <v>2</v>
+      </c>
+      <c r="J92" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B83" t="s">
+      <c r="K92" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C83" t="s">
+      <c r="L92" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="D83" t="s">
+      <c r="M92" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>92</v>
+      </c>
+      <c r="C93" t="s">
+        <v>93</v>
+      </c>
+      <c r="D93" t="s">
+        <v>25</v>
+      </c>
+      <c r="E93" t="s">
+        <v>26</v>
+      </c>
+      <c r="F93" t="s">
+        <v>27</v>
+      </c>
+      <c r="G93"/>
+      <c r="H93" s="7">
+        <v>42229</v>
+      </c>
+      <c r="I93" s="5">
+        <v>10</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K93" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="L93" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="M93" s="5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B94" t="s">
+        <v>143</v>
+      </c>
+      <c r="C94" s="8">
+        <v>42201</v>
+      </c>
+      <c r="D94" t="s">
         <v>19</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E94" t="s">
+        <v>20</v>
+      </c>
+      <c r="F94" t="s">
         <v>27</v>
       </c>
-      <c r="F83" t="s">
+      <c r="G94" t="s">
         <v>30</v>
       </c>
-      <c r="G83" s="7">
-        <v>42277</v>
-      </c>
-      <c r="H83" s="5">
-        <v>5</v>
-      </c>
-      <c r="I83" s="5" t="s">
+      <c r="H94" s="7">
+        <v>42247</v>
+      </c>
+      <c r="I94" s="5">
+        <v>1</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="K94" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="L94" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M94" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="J83" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="K83" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="L83" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B84" t="s">
-        <v>94</v>
-      </c>
-      <c r="C84" s="8">
-        <v>42216</v>
-      </c>
-      <c r="D84" t="s">
-        <v>19</v>
-      </c>
-      <c r="E84" t="s">
-        <v>22</v>
-      </c>
-      <c r="G84" s="7">
-        <v>42247</v>
-      </c>
-      <c r="H84" s="5">
-        <v>2</v>
-      </c>
-      <c r="I84" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J84" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="K84" t="s">
-        <v>97</v>
-      </c>
-      <c r="L84" s="5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" t="s">
-        <v>100</v>
-      </c>
-      <c r="C85" t="s">
-        <v>101</v>
-      </c>
-      <c r="D85" t="s">
-        <v>25</v>
-      </c>
-      <c r="E85" t="s">
-        <v>27</v>
-      </c>
-      <c r="G85" s="7">
-        <v>42229</v>
-      </c>
-      <c r="H85" s="5">
-        <v>10</v>
-      </c>
-      <c r="I85" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="J85" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="K85" t="s">
-        <v>105</v>
-      </c>
-      <c r="L85" s="5" t="s">
-        <v>106</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E41" r:id="rId1"/>
-    <hyperlink ref="E43" r:id="rId2"/>
-    <hyperlink ref="E44" r:id="rId3"/>
-    <hyperlink ref="E45" r:id="rId4"/>
-    <hyperlink ref="E42" r:id="rId5"/>
+    <hyperlink ref="F43" r:id="rId1"/>
+    <hyperlink ref="F45" r:id="rId2"/>
+    <hyperlink ref="F46" r:id="rId3"/>
+    <hyperlink ref="F47" r:id="rId4"/>
+    <hyperlink ref="F44" r:id="rId5"/>
+    <hyperlink ref="F48" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Fixed several display issues, got a lot of Dashboard working
</commit_message>
<xml_diff>
--- a/Aardvark/Template.xlsx
+++ b/Aardvark/Template.xlsx
@@ -919,9 +919,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M139"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G53" activeCellId="2" sqref="G49 G52 G53"/>
+      <selection pane="topRight" activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,7 +951,7 @@
       </c>
       <c r="B2" s="9">
         <f ca="1">NOW()</f>
-        <v>42233.462126736114</v>
+        <v>42238.756730208333</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>